<commit_message>
Update date column in SMR unit roster
</commit_message>
<xml_diff>
--- a/SMR.Extensions/unitRoster.xlsx
+++ b/SMR.Extensions/unitRoster.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\database\SMR.Extensions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\database\SMR.Extensions\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,6 +77,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -140,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -156,6 +159,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="10"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +501,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,6 +512,7 @@
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="5"/>
     <col min="9" max="9" width="9.140625" style="7"/>
+    <col min="15" max="15" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="76.5" customHeight="1">
@@ -573,7 +578,7 @@
       <c r="N3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>